<commit_message>
Change the units for dfba_obj_species
</commit_message>
<xml_diff>
--- a/tests/fixtures/verification/cases/multialgorithmic/00001/00001-wc_lang.xlsx
+++ b/tests/fixtures/verification/cases/multialgorithmic/00001/00001-wc_lang.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-22545" yWindow="11235" windowWidth="22275" windowHeight="9435" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="-22545" yWindow="11235" windowWidth="22275" windowHeight="9435" firstSheet="13" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,9 @@
     <sheet name="!!Authors" sheetId="23" r:id="rId23"/>
     <sheet name="!!Changes" sheetId="24" r:id="rId24"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId25"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Table of contents'!$A$3:$C$27</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">'!!Authors'!$A$2:$L$2</definedName>
@@ -5132,13 +5135,13 @@
     <t>Biomass reaction</t>
   </si>
   <si>
-    <t>molar / second</t>
-  </si>
-  <si>
     <t>dfba-net-species-biomass_reaction-Sink[c]</t>
   </si>
   <si>
     <t>k_cat</t>
+  </si>
+  <si>
+    <t>molecule / cell</t>
   </si>
 </sst>
 </file>
@@ -5340,14 +5343,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -5364,6 +5367,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="!!Submodels"/>
+      <sheetName val="!!Species"/>
+      <sheetName val="!!dFBA objective reactions"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5943,7 +5963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -6365,11 +6385,11 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -7487,9 +7507,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -7550,7 +7570,7 @@
     </row>
     <row r="3" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -7559,11 +7579,11 @@
       <c r="D3" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="29">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -7882,7 +7902,7 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -8256,28 +8276,28 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="29" t="s">
+      <c r="H2" s="31"/>
+      <c r="I2" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
-      <c r="Q2" s="29" t="s">
+      <c r="Q2" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="29" t="s">
+      <c r="R2" s="31"/>
+      <c r="S2" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="T2" s="30"/>
+      <c r="T2" s="31"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
@@ -9152,10 +9172,10 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="H2" s="30"/>
+      <c r="H2" s="31"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -10903,19 +10923,19 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
@@ -11329,14 +11349,14 @@
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>

</xml_diff>